<commit_message>
Agregar csv con dublin core
</commit_message>
<xml_diff>
--- a/data/metadatos-bga.xlsx
+++ b/data/metadatos-bga.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilianaparis/Documents/GitHub/coleccion-bga/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B1E89B-11F9-D442-B640-BB6B9BAC216F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E16048FD-3A54-5B46-91EA-625719D764FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21820" activeTab="1" xr2:uid="{DB73FFB8-DED9-574F-B05E-3295B1C29935}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21820" xr2:uid="{DB73FFB8-DED9-574F-B05E-3295B1C29935}"/>
   </bookViews>
   <sheets>
-    <sheet name="Obra" sheetId="1" r:id="rId1"/>
-    <sheet name="Referentes" sheetId="2" r:id="rId2"/>
+    <sheet name="obras-bga" sheetId="1" r:id="rId1"/>
+    <sheet name="referentes-bga" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,21 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>dimensiones</t>
-  </si>
-  <si>
-    <t>tecnica</t>
-  </si>
-  <si>
     <t>archivo</t>
   </si>
   <si>
@@ -70,9 +55,6 @@
     <t>suicidas-sisga-1.jpg</t>
   </si>
   <si>
-    <t>periodico</t>
-  </si>
-  <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
@@ -131,6 +113,24 @@
   </si>
   <si>
     <t>exmilitar-mata-esposa.jpg</t>
+  </si>
+  <si>
+    <t>dc.title</t>
+  </si>
+  <si>
+    <t>dc.date</t>
+  </si>
+  <si>
+    <t>dc.publisher</t>
+  </si>
+  <si>
+    <t>dc.identifier</t>
+  </si>
+  <si>
+    <t>dc.format</t>
+  </si>
+  <si>
+    <t>dc.medium</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17047F3B-1152-B54A-B017-62D571EE9E2A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,22 +500,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -523,19 +523,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -543,19 +543,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -563,19 +563,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6282ED-0426-254B-B84C-A696ED5B28F2}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,19 +601,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -621,16 +621,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -638,16 +638,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -655,10 +655,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -666,10 +666,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>